<commit_message>
Add new checks (240/3)
</commit_message>
<xml_diff>
--- a/hitt/HITT checks summary.xlsx
+++ b/hitt/HITT checks summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\github\helix-tools\hitt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE3C571-0362-4FFA-83A6-79D401EF6986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1686671A-9698-4866-96DB-CAC36E415A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14685" yWindow="3075" windowWidth="58470" windowHeight="17100" xr2:uid="{410C6642-7ACB-475F-8776-3B5E3A576498}"/>
+    <workbookView xWindow="34065" yWindow="360" windowWidth="42210" windowHeight="17580" xr2:uid="{410C6642-7ACB-475F-8776-3B5E3A576498}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="158">
   <si>
     <t>#</t>
   </si>
@@ -501,6 +501,18 @@
   </si>
   <si>
     <t>Check for OS binaries - python dos2unix etc</t>
+  </si>
+  <si>
+    <t>DB_PORT not blank</t>
+  </si>
+  <si>
+    <t>IMAGESECRET_NAME not blank</t>
+  </si>
+  <si>
+    <t>The HELIX_FULL_STACK_UPGRADE option sbould not be selected when the DEPLOYMENT_MODE is UPDATE</t>
+  </si>
+  <si>
+    <t>HELIX_FULL_STACK_UPGRADE is not selected but it is required when the DEPLOYMENT_MODE is UPGRADE</t>
   </si>
 </sst>
 </file>
@@ -900,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C127526-6982-42DF-8CA7-3E3577A646DB}">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+      <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,6 +2800,62 @@
         <v>136</v>
       </c>
     </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>240</v>
+      </c>
+      <c r="B138" t="s">
+        <v>154</v>
+      </c>
+      <c r="C138" t="s">
+        <v>127</v>
+      </c>
+      <c r="D138" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>241</v>
+      </c>
+      <c r="B139" t="s">
+        <v>157</v>
+      </c>
+      <c r="C139" t="s">
+        <v>127</v>
+      </c>
+      <c r="D139" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>242</v>
+      </c>
+      <c r="B140" t="s">
+        <v>156</v>
+      </c>
+      <c r="C140" t="s">
+        <v>127</v>
+      </c>
+      <c r="D140" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>243</v>
+      </c>
+      <c r="B141" t="s">
+        <v>155</v>
+      </c>
+      <c r="C141" t="s">
+        <v>127</v>
+      </c>
+      <c r="D141" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update list of checks
</commit_message>
<xml_diff>
--- a/hitt/HITT checks summary.xlsx
+++ b/hitt/HITT checks summary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\github\helix-tools\hitt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934F6B23-E50A-4F64-9577-00A6CCF613CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162361C4-EE5C-43AA-B762-A9F5C064C758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28710" yWindow="2490" windowWidth="44625" windowHeight="17505" xr2:uid="{410C6642-7ACB-475F-8776-3B5E3A576498}"/>
+    <workbookView xWindow="17895" yWindow="3915" windowWidth="28560" windowHeight="14130" xr2:uid="{410C6642-7ACB-475F-8776-3B5E3A576498}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$152</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="162">
   <si>
     <t>#</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>Git repo directory name match for global libraries</t>
+  </si>
+  <si>
+    <t>SSH setup checks</t>
+  </si>
+  <si>
+    <t>Pipeline library trailing space check</t>
   </si>
 </sst>
 </file>
@@ -921,11 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C127526-6982-42DF-8CA7-3E3577A646DB}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D145" sqref="D145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,12 +954,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -968,7 +973,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1010,7 +1015,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1024,7 +1029,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1038,7 +1043,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1052,7 +1057,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -1080,7 +1085,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>13</v>
       </c>
@@ -1094,7 +1099,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -1108,7 +1113,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -1122,7 +1127,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16</v>
       </c>
@@ -1136,7 +1141,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17</v>
       </c>
@@ -1150,7 +1155,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>18</v>
       </c>
@@ -1164,7 +1169,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>19</v>
       </c>
@@ -1178,7 +1183,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -1192,7 +1197,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>22</v>
       </c>
@@ -1206,7 +1211,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>24</v>
       </c>
@@ -1220,7 +1225,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>25</v>
       </c>
@@ -1234,7 +1239,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>26</v>
       </c>
@@ -1248,7 +1253,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>31</v>
       </c>
@@ -1262,7 +1267,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>33</v>
       </c>
@@ -1276,7 +1281,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>34</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>35</v>
       </c>
@@ -1318,7 +1323,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>101</v>
       </c>
@@ -1332,7 +1337,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>102</v>
       </c>
@@ -1346,7 +1351,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>103</v>
       </c>
@@ -1360,7 +1365,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>104</v>
       </c>
@@ -1374,7 +1379,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>106</v>
       </c>
@@ -1388,7 +1393,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>107</v>
       </c>
@@ -1402,7 +1407,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>110</v>
       </c>
@@ -1413,7 +1418,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>111</v>
       </c>
@@ -1441,7 +1446,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>113</v>
       </c>
@@ -1469,7 +1474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>115</v>
       </c>
@@ -1553,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>121</v>
       </c>
@@ -1567,7 +1572,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>122</v>
       </c>
@@ -1581,7 +1586,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>124</v>
       </c>
@@ -1595,7 +1600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>125</v>
       </c>
@@ -1609,7 +1614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>126</v>
       </c>
@@ -1623,7 +1628,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>127</v>
       </c>
@@ -1637,7 +1642,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>131</v>
       </c>
@@ -1651,7 +1656,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>132</v>
       </c>
@@ -1665,7 +1670,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>133</v>
       </c>
@@ -1679,7 +1684,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>134</v>
       </c>
@@ -1693,7 +1698,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>135</v>
       </c>
@@ -1707,7 +1712,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>137</v>
       </c>
@@ -1721,7 +1726,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>139</v>
       </c>
@@ -1735,7 +1740,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>141</v>
       </c>
@@ -1749,7 +1754,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>142</v>
       </c>
@@ -1763,7 +1768,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>143</v>
       </c>
@@ -1777,7 +1782,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>144</v>
       </c>
@@ -1791,7 +1796,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>145</v>
       </c>
@@ -1805,7 +1810,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>146</v>
       </c>
@@ -1819,7 +1824,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>147</v>
       </c>
@@ -1833,7 +1838,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>148</v>
       </c>
@@ -1847,7 +1852,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>149</v>
       </c>
@@ -1861,7 +1866,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>150</v>
       </c>
@@ -1875,7 +1880,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>151</v>
       </c>
@@ -1889,7 +1894,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>152</v>
       </c>
@@ -1903,7 +1908,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>153</v>
       </c>
@@ -1917,7 +1922,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>154</v>
       </c>
@@ -1931,7 +1936,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>155</v>
       </c>
@@ -1945,7 +1950,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>156</v>
       </c>
@@ -1959,7 +1964,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>157</v>
       </c>
@@ -1973,7 +1978,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>158</v>
       </c>
@@ -1987,7 +1992,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>159</v>
       </c>
@@ -2001,7 +2006,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>160</v>
       </c>
@@ -2015,7 +2020,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>161</v>
       </c>
@@ -2029,7 +2034,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>162</v>
       </c>
@@ -2043,7 +2048,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>163</v>
       </c>
@@ -2057,7 +2062,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>164</v>
       </c>
@@ -2071,7 +2076,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>165</v>
       </c>
@@ -2085,7 +2090,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>166</v>
       </c>
@@ -2099,7 +2104,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>167</v>
       </c>
@@ -2113,7 +2118,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>168</v>
       </c>
@@ -2127,7 +2132,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>169</v>
       </c>
@@ -2141,7 +2146,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>170</v>
       </c>
@@ -2155,7 +2160,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>171</v>
       </c>
@@ -2169,7 +2174,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>172</v>
       </c>
@@ -2183,7 +2188,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>173</v>
       </c>
@@ -2197,7 +2202,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>174</v>
       </c>
@@ -2211,7 +2216,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>175</v>
       </c>
@@ -2225,7 +2230,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>177</v>
       </c>
@@ -2239,7 +2244,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>178</v>
       </c>
@@ -2253,7 +2258,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>179</v>
       </c>
@@ -2267,7 +2272,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>181</v>
       </c>
@@ -2281,7 +2286,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>182</v>
       </c>
@@ -2295,7 +2300,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>183</v>
       </c>
@@ -2309,7 +2314,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>185</v>
       </c>
@@ -2323,7 +2328,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>186</v>
       </c>
@@ -2337,7 +2342,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>192</v>
       </c>
@@ -2351,7 +2356,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>193</v>
       </c>
@@ -2365,7 +2370,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>194</v>
       </c>
@@ -2379,7 +2384,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>195</v>
       </c>
@@ -2393,7 +2398,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>196</v>
       </c>
@@ -2407,7 +2412,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>197</v>
       </c>
@@ -2421,7 +2426,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>201</v>
       </c>
@@ -2435,7 +2440,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>205</v>
       </c>
@@ -2449,7 +2454,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>208</v>
       </c>
@@ -2463,7 +2468,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>209</v>
       </c>
@@ -2477,7 +2482,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>212</v>
       </c>
@@ -2491,7 +2496,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>213</v>
       </c>
@@ -2505,7 +2510,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>214</v>
       </c>
@@ -2519,7 +2524,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>215</v>
       </c>
@@ -2533,7 +2538,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>217</v>
       </c>
@@ -2547,7 +2552,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>218</v>
       </c>
@@ -2561,7 +2566,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>220</v>
       </c>
@@ -2575,7 +2580,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>221</v>
       </c>
@@ -2589,7 +2594,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>222</v>
       </c>
@@ -2603,7 +2608,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>223</v>
       </c>
@@ -2617,7 +2622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>224</v>
       </c>
@@ -2631,7 +2636,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>225</v>
       </c>
@@ -2645,7 +2650,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>226</v>
       </c>
@@ -2673,7 +2678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>230</v>
       </c>
@@ -2687,7 +2692,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>231</v>
       </c>
@@ -2715,7 +2720,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>233</v>
       </c>
@@ -2729,7 +2734,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>234</v>
       </c>
@@ -2743,7 +2748,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>235</v>
       </c>
@@ -2757,7 +2762,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>236</v>
       </c>
@@ -2771,7 +2776,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>237</v>
       </c>
@@ -2785,7 +2790,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>238</v>
       </c>
@@ -2799,7 +2804,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>239</v>
       </c>
@@ -2813,7 +2818,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>240</v>
       </c>
@@ -2827,7 +2832,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>241</v>
       </c>
@@ -2841,7 +2846,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>242</v>
       </c>
@@ -2855,7 +2860,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>243</v>
       </c>
@@ -2869,7 +2874,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>244</v>
       </c>
@@ -2883,12 +2888,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>245</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>246</v>
       </c>
@@ -2902,14 +2907,36 @@
         <v>139</v>
       </c>
     </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>247</v>
+      </c>
+      <c r="B143" t="s">
+        <v>160</v>
+      </c>
+      <c r="C143" t="s">
+        <v>129</v>
+      </c>
+      <c r="D143" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>248</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C144" t="s">
+        <v>127</v>
+      </c>
+      <c r="D144" t="s">
+        <v>139</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D142" xr:uid="{9C127526-6982-42DF-8CA7-3E3577A646DB}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="RSSO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D152" xr:uid="{9C127526-6982-42DF-8CA7-3E3577A646DB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>